<commit_message>
create acceptance criteria of backlog for sprint 1
</commit_message>
<xml_diff>
--- a/docs/acceptance-tests.xlsx
+++ b/docs/acceptance-tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6368a6be5aca3f60/Documents/HTL/WMC/room-food/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{44113145-4501-44D9-A1EB-8D4ED0044DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="8_{44113145-4501-44D9-A1EB-8D4ED0044DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD09A589-70BB-464C-B43C-36EB7F4452AC}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8D6859AF-9A25-468C-BEF1-C20AEB03BB66}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{8D6859AF-9A25-468C-BEF1-C20AEB03BB66}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,10 +35,92 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+  <si>
+    <t>backlog item</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>acceptance criteria</t>
+  </si>
+  <si>
+    <t>create a basic add meal functionality</t>
+  </si>
+  <si>
+    <t>create a basic login</t>
+  </si>
+  <si>
+    <t>create a basic page for a room preview</t>
+  </si>
+  <si>
+    <t>frontend and routes for basic login</t>
+  </si>
+  <si>
+    <t>always accessable database, read/write access, store account info securely, functional backend</t>
+  </si>
+  <si>
+    <t>frontend and routes for adding a meal</t>
+  </si>
+  <si>
+    <t>backend service and database for meals</t>
+  </si>
+  <si>
+    <t>store meals of each room, read/write access</t>
+  </si>
+  <si>
+    <t>frontend and routes for room view</t>
+  </si>
+  <si>
+    <t>backend service and database for room view</t>
+  </si>
+  <si>
+    <t>backend service and database for basic login</t>
+  </si>
+  <si>
+    <t>login page, working connection to backend, register/log in/delete account functionality</t>
+  </si>
+  <si>
+    <t>sprint 1</t>
+  </si>
+  <si>
+    <t>general</t>
+  </si>
+  <si>
+    <t>popup for adding a meal which provides fields for name, meal type (dropdown), description and date/time</t>
+  </si>
+  <si>
+    <t>should be able to fetch mealplans from the database, no editing yet</t>
+  </si>
+  <si>
+    <t>display sortable overview of meals planned in the current room, should update when new meals are added, meals should be clickable which opens up a popup with the details</t>
+  </si>
+  <si>
+    <t>satisfy criteria of #18 and #19</t>
+  </si>
+  <si>
+    <t>satisfy criteria of #20, #21 and #9,</t>
+  </si>
+  <si>
+    <t>satisfy criteria of #15 and #17</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -66,8 +148,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -402,12 +486,152 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27CE6F7A-6338-4811-9608-87890EA30097}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5546875" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:C11">
+    <sortCondition ref="A4:A11"/>
+  </sortState>
+  <mergeCells count="2">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A12:C12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
separate acceptance tests for sprint 1, edit file name
</commit_message>
<xml_diff>
--- a/docs/acceptance-tests.xlsx
+++ b/docs/acceptance-tests.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6368a6be5aca3f60/Documents/HTL/WMC/room-food/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="120" documentId="8_{44113145-4501-44D9-A1EB-8D4ED0044DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0010897-7B3E-4C50-99BA-4367555C07A3}"/>
+  <xr:revisionPtr revIDLastSave="144" documentId="8_{44113145-4501-44D9-A1EB-8D4ED0044DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{574764D3-D1E7-4715-9E73-9810E68D39D3}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8D6859AF-9A25-468C-BEF1-C20AEB03BB66}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{8D6859AF-9A25-468C-BEF1-C20AEB03BB66}"/>
   </bookViews>
   <sheets>
-    <sheet name="acceptance-tests" sheetId="1" r:id="rId1"/>
+    <sheet name="All Tests" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint 1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,17 +37,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
-  <si>
-    <t>backlog item</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>#</t>
   </si>
   <si>
-    <t>acceptance criteria</t>
-  </si>
-  <si>
     <t>create a basic add meal functionality</t>
   </si>
   <si>
@@ -68,9 +63,6 @@
     <t>backend service and database for meals</t>
   </si>
   <si>
-    <t>store meals of each room, read/write access</t>
-  </si>
-  <si>
     <t>frontend and routes for room view</t>
   </si>
   <si>
@@ -83,18 +75,9 @@
     <t>login page, working connection to backend, register/log in/delete account functionality</t>
   </si>
   <si>
-    <t>sprint 1</t>
-  </si>
-  <si>
-    <t>general</t>
-  </si>
-  <si>
     <t>popup for adding a meal which provides fields for name, meal type (dropdown), description and date/time</t>
   </si>
   <si>
-    <t>should be able to fetch mealplans from the database, no editing yet</t>
-  </si>
-  <si>
     <t>display sortable overview of meals planned in the current room, should update when new meals are added, meals should be clickable which opens up a popup with the details</t>
   </si>
   <si>
@@ -177,6 +160,18 @@
   </si>
   <si>
     <t>create a "new recipe" popup</t>
+  </si>
+  <si>
+    <t>Backlog Item</t>
+  </si>
+  <si>
+    <t>Acceptance Criteria</t>
+  </si>
+  <si>
+    <t>store meals of each user, read/write access</t>
+  </si>
+  <si>
+    <t>should be able to fetch meal plans from the database, no editing yet</t>
   </si>
 </sst>
 </file>
@@ -220,9 +215,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -558,11 +552,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27CE6F7A-6338-4811-9608-87890EA30097}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -574,268 +568,281 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>14</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C12">
+    <sortCondition ref="A2:A12"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7B459D0-6ACC-4847-ACE5-9F58AF7160CD}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
         <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>20</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>21</v>
-      </c>
-      <c r="B11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>4</v>
-      </c>
-      <c r="B13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>5</v>
-      </c>
-      <c r="B14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>6</v>
-      </c>
-      <c r="B15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <v>7</v>
-      </c>
-      <c r="B16" t="s">
-        <v>26</v>
-      </c>
-      <c r="C16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>8</v>
-      </c>
-      <c r="B17" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <v>10</v>
-      </c>
-      <c r="B18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>11</v>
-      </c>
-      <c r="B19" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>12</v>
-      </c>
-      <c r="B20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>13</v>
-      </c>
-      <c r="B21" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <v>14</v>
-      </c>
-      <c r="B22" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <v>16</v>
-      </c>
-      <c r="B23" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" t="s">
-        <v>45</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A13:C23">
-    <sortCondition ref="A13:A23"/>
-  </sortState>
-  <mergeCells count="2">
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A12:C12"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
upload presentation, edit acceptance tests
</commit_message>
<xml_diff>
--- a/docs/acceptance-tests.xlsx
+++ b/docs/acceptance-tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6368a6be5aca3f60/Documents/HTL/WMC/room-food/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="144" documentId="8_{44113145-4501-44D9-A1EB-8D4ED0044DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{574764D3-D1E7-4715-9E73-9810E68D39D3}"/>
+  <xr:revisionPtr revIDLastSave="156" documentId="8_{44113145-4501-44D9-A1EB-8D4ED0044DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96A1B935-AD95-4CE0-A059-FEBD74AD901D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{8D6859AF-9A25-468C-BEF1-C20AEB03BB66}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8D6859AF-9A25-468C-BEF1-C20AEB03BB66}"/>
   </bookViews>
   <sheets>
     <sheet name="All Tests" sheetId="1" r:id="rId1"/>
@@ -132,9 +132,6 @@
     <t xml:space="preserve">satisfy criteria of #8, should list all assigned ingredients needed for planned meals, user should be able to add/edit/remove additional items, </t>
   </si>
   <si>
-    <t>satisfy criteria of #14, when creating a meal, user should be able to choose from saved or public recipes or create a new recipe, a recipe should contain a list of ingredients, steps of preparation (description) and time to prepare, a recipe should be able to be set to either private or public, a recipe should be able to be shared per link</t>
-  </si>
-  <si>
     <t>satisfy criteria of #4 and #22, a profile should have a username, full name, date of birth, about me, participating rooms and a profile picture, the user should be able to choose what they want to make public, the information should be stored in the database and editable</t>
   </si>
   <si>
@@ -147,9 +144,6 @@
     <t>satisfy criteria of #13, a user should be able to modify the data of any room theyre the owner of and invite/kick users</t>
   </si>
   <si>
-    <t>a room owner should be able to invite people by invite link or username, users should be able to request to join a room by entering the room code or searching for rooms on the website, the room owner should be able to accept or deny the request and the user should be able to see pending requests</t>
-  </si>
-  <si>
     <t>satisfy criteria of #16, a user creating a meal plan should be able to choose a saved recipe or search for a public recipe</t>
   </si>
   <si>
@@ -172,6 +166,12 @@
   </si>
   <si>
     <t>should be able to fetch meal plans from the database, no editing yet</t>
+  </si>
+  <si>
+    <t>a room owner should be able to invite people by invite link or username, users should be able to request to join a room by entering the room code or searching for rooms, the room owner should be able to accept or deny the request and the user should be able to see pending requests</t>
+  </si>
+  <si>
+    <t>satisfy criteria of #14, when creating a meal, a user should be able to choose from saved or public recipes or create a new recipe, a recipe should contain a list of ingredients, steps of preparation (description) and time to prepare, a recipe should be either private or public, a recipe should be able to be shared per link</t>
   </si>
 </sst>
 </file>
@@ -554,16 +554,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27CE6F7A-6338-4811-9608-87890EA30097}">
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomLeft" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.5546875" customWidth="1"/>
-    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="2" max="2" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="254.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -571,10 +571,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -596,7 +596,7 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -629,7 +629,7 @@
         <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -640,7 +640,7 @@
         <v>22</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -651,7 +651,7 @@
         <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -662,7 +662,7 @@
         <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -673,7 +673,7 @@
         <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -684,7 +684,7 @@
         <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -695,7 +695,7 @@
         <v>27</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -703,10 +703,10 @@
         <v>22</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -721,15 +721,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7B459D0-6ACC-4847-ACE5-9F58AF7160CD}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.109375" customWidth="1"/>
+    <col min="2" max="2" width="37.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="140.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -737,10 +738,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -806,7 +807,7 @@
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -839,7 +840,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create all pdfs, upload screenshot of backlog
</commit_message>
<xml_diff>
--- a/docs/acceptance-tests.xlsx
+++ b/docs/acceptance-tests.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6368a6be5aca3f60/Documents/HTL/WMC/room-food/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="156" documentId="8_{44113145-4501-44D9-A1EB-8D4ED0044DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96A1B935-AD95-4CE0-A059-FEBD74AD901D}"/>
+  <xr:revisionPtr revIDLastSave="164" documentId="8_{44113145-4501-44D9-A1EB-8D4ED0044DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37085657-5CE5-435C-AD87-8C2E7698B10D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8D6859AF-9A25-468C-BEF1-C20AEB03BB66}"/>
   </bookViews>
@@ -552,6 +552,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27CE6F7A-6338-4811-9608-87890EA30097}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -713,12 +716,16 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C12">
     <sortCondition ref="A2:A12"/>
   </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="8" scale="70" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7B459D0-6ACC-4847-ACE5-9F58AF7160CD}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -845,5 +852,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="72" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>